<commit_message>
Refactor LinearizerAbsTaylor to use SA.v1 instead of SA.v7 for parallelization
</commit_message>
<xml_diff>
--- a/Trabajo/Data/combined_averages.xlsx
+++ b/Trabajo/Data/combined_averages.xlsx
@@ -495,7 +495,7 @@
         <v>1.58</v>
       </c>
       <c r="G2">
-        <v>6.37</v>
+        <v>3.23</v>
       </c>
       <c r="H2">
         <v>8.32</v>
@@ -521,7 +521,7 @@
         <v>59.33</v>
       </c>
       <c r="G3">
-        <v>71</v>
+        <v>75.26000000000001</v>
       </c>
       <c r="H3">
         <v>76.62</v>
@@ -547,7 +547,7 @@
         <v>18.49</v>
       </c>
       <c r="G4">
-        <v>11.02</v>
+        <v>16.23</v>
       </c>
       <c r="H4">
         <v>8.76</v>
@@ -573,7 +573,7 @@
         <v>14.64</v>
       </c>
       <c r="G5">
-        <v>9.710000000000001</v>
+        <v>12.5</v>
       </c>
       <c r="H5">
         <v>7.95</v>
@@ -599,7 +599,7 @@
         <v>9.58</v>
       </c>
       <c r="G6">
-        <v>9.619999999999999</v>
+        <v>13.03</v>
       </c>
       <c r="H6">
         <v>12.03</v>
@@ -625,7 +625,7 @@
         <v>15.7</v>
       </c>
       <c r="G7">
-        <v>17.52</v>
+        <v>23.54</v>
       </c>
       <c r="H7">
         <v>13.65</v>
@@ -651,7 +651,7 @@
         <v>0.6</v>
       </c>
       <c r="G8">
-        <v>1.13</v>
+        <v>1.11</v>
       </c>
       <c r="H8">
         <v>1.33</v>
@@ -677,7 +677,7 @@
         <v>63.05</v>
       </c>
       <c r="G9">
-        <v>77</v>
+        <v>153.04</v>
       </c>
       <c r="H9">
         <v>114.79</v>
@@ -703,7 +703,7 @@
         <v>28.57</v>
       </c>
       <c r="G10">
-        <v>39.26</v>
+        <v>54.18</v>
       </c>
       <c r="H10">
         <v>50.13</v>
@@ -728,6 +728,9 @@
       <c r="F11">
         <v>1.66</v>
       </c>
+      <c r="G11">
+        <v>3.99</v>
+      </c>
       <c r="H11">
         <v>157.92</v>
       </c>
@@ -751,6 +754,9 @@
       <c r="F12">
         <v>1.39</v>
       </c>
+      <c r="G12">
+        <v>2.93</v>
+      </c>
       <c r="H12">
         <v>58.08</v>
       </c>
@@ -775,7 +781,7 @@
         <v>0.66</v>
       </c>
       <c r="G13">
-        <v>2.67</v>
+        <v>1.16</v>
       </c>
       <c r="H13">
         <v>9.449999999999999</v>
@@ -801,7 +807,7 @@
         <v>29.96</v>
       </c>
       <c r="G14">
-        <v>9.960000000000001</v>
+        <v>87.01000000000001</v>
       </c>
       <c r="H14">
         <v>7.26</v>
@@ -931,7 +937,7 @@
         <v>589.6</v>
       </c>
       <c r="G2">
-        <v>2348.8</v>
+        <v>632.8</v>
       </c>
       <c r="H2">
         <v>2348.8</v>
@@ -957,7 +963,7 @@
         <v>12582.4</v>
       </c>
       <c r="G3">
-        <v>18262</v>
+        <v>12119.6</v>
       </c>
       <c r="H3">
         <v>18262</v>
@@ -983,7 +989,7 @@
         <v>1606.4</v>
       </c>
       <c r="G4">
-        <v>1614</v>
+        <v>1653.6</v>
       </c>
       <c r="H4">
         <v>1614</v>
@@ -1009,7 +1015,7 @@
         <v>5209.6</v>
       </c>
       <c r="G5">
-        <v>5169.2</v>
+        <v>5108.4</v>
       </c>
       <c r="H5">
         <v>5169.2</v>
@@ -1035,7 +1041,7 @@
         <v>5150.8</v>
       </c>
       <c r="G6">
-        <v>5114</v>
+        <v>5081.6</v>
       </c>
       <c r="H6">
         <v>5114</v>
@@ -1061,7 +1067,7 @@
         <v>11300</v>
       </c>
       <c r="G7">
-        <v>11170</v>
+        <v>11185.2</v>
       </c>
       <c r="H7">
         <v>11170</v>
@@ -1087,7 +1093,7 @@
         <v>264.8</v>
       </c>
       <c r="G8">
-        <v>490</v>
+        <v>239.6</v>
       </c>
       <c r="H8">
         <v>490</v>
@@ -1113,7 +1119,7 @@
         <v>60171.2</v>
       </c>
       <c r="G9">
-        <v>60305.6</v>
+        <v>60294.8</v>
       </c>
       <c r="H9">
         <v>60305.6</v>
@@ -1139,7 +1145,7 @@
         <v>31808.4</v>
       </c>
       <c r="G10">
-        <v>31837</v>
+        <v>31781.2</v>
       </c>
       <c r="H10">
         <v>31831.6</v>
@@ -1164,6 +1170,9 @@
       <c r="F11">
         <v>422.4</v>
       </c>
+      <c r="G11">
+        <v>500</v>
+      </c>
       <c r="H11">
         <v>39850.67</v>
       </c>
@@ -1187,6 +1196,9 @@
       <c r="F12">
         <v>991.6</v>
       </c>
+      <c r="G12">
+        <v>999.2</v>
+      </c>
       <c r="H12">
         <v>23447.2</v>
       </c>
@@ -1211,7 +1223,7 @@
         <v>161.2</v>
       </c>
       <c r="G13">
-        <v>821.33</v>
+        <v>153.6</v>
       </c>
       <c r="H13">
         <v>3054</v>
@@ -1237,7 +1249,7 @@
         <v>3173.6</v>
       </c>
       <c r="G14">
-        <v>843.2</v>
+        <v>2771.6</v>
       </c>
       <c r="H14">
         <v>843.2</v>
@@ -1254,11 +1266,6 @@
       <formula>NOT(ISERROR(B3))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="notContainsErrors" dxfId="0" priority="4">
-      <formula>NOT(ISERROR(B5))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B7">
     <cfRule type="notContainsErrors" dxfId="0" priority="6">
       <formula>NOT(ISERROR(B7))</formula>
@@ -1269,11 +1276,6 @@
       <formula>NOT(ISERROR(C12))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="notContainsErrors" dxfId="0" priority="5">
-      <formula>NOT(ISERROR(C6))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E10">
     <cfRule type="notContainsErrors" dxfId="0" priority="9">
       <formula>NOT(ISERROR(E10))</formula>
@@ -1284,11 +1286,6 @@
       <formula>NOT(ISERROR(E14))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="notContainsErrors" dxfId="0" priority="7">
-      <formula>NOT(ISERROR(E8))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E9">
     <cfRule type="notContainsErrors" dxfId="0" priority="8">
       <formula>NOT(ISERROR(E9))</formula>
@@ -1309,6 +1306,21 @@
       <formula>NOT(ISERROR(F4))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="notContainsErrors" dxfId="0" priority="4">
+      <formula>NOT(ISERROR(G5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="notContainsErrors" dxfId="0" priority="5">
+      <formula>NOT(ISERROR(G6))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="notContainsErrors" dxfId="0" priority="7">
+      <formula>NOT(ISERROR(G8))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>